<commit_message>
Fix registration data and add graphs of data
</commit_message>
<xml_diff>
--- a/exploration/TeamsCode_Registration_Data/MIHS/Fall_2018_MIHS_Registration.xlsx
+++ b/exploration/TeamsCode_Registration_Data/MIHS/Fall_2018_MIHS_Registration.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AlanBi/Desktop/TeamsCode/Registration Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AlanBi/Desktop/App Development/Python/PythonSelfStudy/exploration/TeamsCode_Registration_Data/MIHS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9603CC60-EC96-9347-96A2-86F86393FC36}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18919F15-A72C-3541-9BE2-E8ADD41E47DE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="104">
   <si>
     <t>Language</t>
   </si>
@@ -41,9 +41,6 @@
     <t>HW</t>
   </si>
   <si>
-    <t xml:space="preserve">Evergreen Middle School </t>
-  </si>
-  <si>
     <t>Java</t>
   </si>
   <si>
@@ -173,9 +170,6 @@
     <t>Yes Buddy</t>
   </si>
   <si>
-    <t xml:space="preserve">Skyline High School </t>
-  </si>
-  <si>
     <t>C#</t>
   </si>
   <si>
@@ -185,9 +179,6 @@
     <t>SSS</t>
   </si>
   <si>
-    <t xml:space="preserve">Issaquah High School </t>
-  </si>
-  <si>
     <t>Team Delta</t>
   </si>
   <si>
@@ -212,9 +203,6 @@
     <t>Ez</t>
   </si>
   <si>
-    <t xml:space="preserve">Tesla STEM High School </t>
-  </si>
-  <si>
     <t>Richmond High Coding Club</t>
   </si>
   <si>
@@ -311,9 +299,6 @@
     <t>Issaquah Middle School, Issaquah High School</t>
   </si>
   <si>
-    <t xml:space="preserve">Eastside Preparatory School </t>
-  </si>
-  <si>
     <t>Interlake High School, Tesla STEM High School</t>
   </si>
   <si>
@@ -339,6 +324,15 @@
   </si>
   <si>
     <t>Newport High School, Tyee Middle School</t>
+  </si>
+  <si>
+    <t>Evergreen Middle School</t>
+  </si>
+  <si>
+    <t>Eastside Preparatory School</t>
+  </si>
+  <si>
+    <t>Skyline High School</t>
   </si>
 </sst>
 </file>
@@ -748,8 +742,8 @@
   <dimension ref="A1:AG72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E65" sqref="E65"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -765,16 +759,16 @@
   <sheetData>
     <row r="1" spans="1:33" ht="15.75" customHeight="1">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -836,10 +830,10 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>101</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:33" ht="15.75" customHeight="1">
@@ -847,16 +841,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>10</v>
-      </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:33" ht="15.75" customHeight="1">
@@ -864,16 +858,16 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:33" ht="15.75" customHeight="1">
@@ -881,16 +875,16 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:33" ht="15.75" customHeight="1">
@@ -898,13 +892,13 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
         <v>4</v>
@@ -915,16 +909,16 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:33" ht="15.75" customHeight="1">
@@ -932,16 +926,16 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
         <v>16</v>
       </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>17</v>
-      </c>
       <c r="E9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:33" ht="15.75" customHeight="1">
@@ -949,7 +943,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
@@ -966,16 +960,16 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:33" ht="15.75" customHeight="1">
@@ -989,10 +983,10 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:33" ht="15.75" customHeight="1">
@@ -1000,16 +994,16 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
         <v>21</v>
       </c>
-      <c r="C13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>22</v>
-      </c>
       <c r="E13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:33" ht="15.75" customHeight="1">
@@ -1017,16 +1011,16 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="E14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:33" ht="15.75" customHeight="1">
@@ -1034,16 +1028,16 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:33" ht="15.75" customHeight="1">
@@ -1051,16 +1045,16 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
         <v>25</v>
       </c>
-      <c r="C16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" t="s">
-        <v>26</v>
-      </c>
       <c r="E16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1">
@@ -1068,16 +1062,16 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
         <v>27</v>
       </c>
-      <c r="C17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" t="s">
-        <v>28</v>
-      </c>
       <c r="E17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1">
@@ -1085,16 +1079,16 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s">
         <v>2</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1">
@@ -1102,16 +1096,16 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
         <v>9</v>
       </c>
-      <c r="D19" t="s">
-        <v>10</v>
-      </c>
       <c r="E19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1">
@@ -1119,16 +1113,16 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1">
@@ -1136,13 +1130,13 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E21" t="s">
         <v>4</v>
@@ -1153,16 +1147,16 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22" t="s">
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1">
@@ -1170,16 +1164,16 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
         <v>34</v>
       </c>
-      <c r="C23" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" t="s">
-        <v>35</v>
-      </c>
       <c r="E23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1">
@@ -1187,16 +1181,16 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" t="s">
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1">
@@ -1204,13 +1198,13 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E25" t="s">
         <v>4</v>
@@ -1221,16 +1215,16 @@
         <v>2</v>
       </c>
       <c r="B26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
         <v>38</v>
       </c>
-      <c r="C26" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" t="s">
-        <v>39</v>
-      </c>
       <c r="E26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1">
@@ -1238,13 +1232,13 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C27" t="s">
         <v>2</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E27" t="s">
         <v>4</v>
@@ -1255,16 +1249,16 @@
         <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C28" t="s">
         <v>2</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1">
@@ -1272,16 +1266,16 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
         <v>42</v>
       </c>
-      <c r="C29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D29" t="s">
-        <v>43</v>
-      </c>
       <c r="E29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1">
@@ -1289,13 +1283,13 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C30" t="s">
         <v>2</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E30" t="s">
         <v>4</v>
@@ -1306,16 +1300,16 @@
         <v>2</v>
       </c>
       <c r="B31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" t="s">
         <v>45</v>
       </c>
-      <c r="C31" t="s">
-        <v>9</v>
-      </c>
-      <c r="D31" t="s">
-        <v>46</v>
-      </c>
       <c r="E31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1">
@@ -1323,16 +1317,16 @@
         <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1">
@@ -1340,16 +1334,16 @@
         <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C33" t="s">
         <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E33" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" customHeight="1">
@@ -1357,16 +1351,16 @@
         <v>3</v>
       </c>
       <c r="B34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" t="s">
+        <v>103</v>
+      </c>
+      <c r="E34" t="s">
         <v>49</v>
-      </c>
-      <c r="C34" t="s">
-        <v>9</v>
-      </c>
-      <c r="D34" t="s">
-        <v>50</v>
-      </c>
-      <c r="E34" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" customHeight="1">
@@ -1374,16 +1368,16 @@
         <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C35" t="s">
         <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E35" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15.75" customHeight="1">
@@ -1391,16 +1385,16 @@
         <v>3</v>
       </c>
       <c r="B36" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C36" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D36" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="E36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15.75" customHeight="1">
@@ -1408,16 +1402,16 @@
         <v>3</v>
       </c>
       <c r="B37" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C37" t="s">
         <v>2</v>
       </c>
       <c r="D37" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E37" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15.75" customHeight="1">
@@ -1425,16 +1419,16 @@
         <v>3</v>
       </c>
       <c r="B38" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D38" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E38" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1">
@@ -1442,16 +1436,16 @@
         <v>3</v>
       </c>
       <c r="B39" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C39" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D39" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" t="s">
         <v>56</v>
-      </c>
-      <c r="E39" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15.75" customHeight="1">
@@ -1459,13 +1453,13 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E40" t="s">
         <v>4</v>
@@ -1476,16 +1470,16 @@
         <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C41" t="s">
         <v>2</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E41" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15.75" customHeight="1">
@@ -1493,16 +1487,16 @@
         <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C42" t="s">
         <v>2</v>
       </c>
       <c r="D42" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E42" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15.75" customHeight="1">
@@ -1510,13 +1504,13 @@
         <v>2</v>
       </c>
       <c r="B43" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C43" t="s">
         <v>2</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E43" t="s">
         <v>4</v>
@@ -1527,16 +1521,16 @@
         <v>3</v>
       </c>
       <c r="B44" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C44" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E44" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="13">
@@ -1544,16 +1538,16 @@
         <v>3</v>
       </c>
       <c r="B45" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C45" t="s">
         <v>2</v>
       </c>
       <c r="D45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E45" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="13">
@@ -1561,16 +1555,16 @@
         <v>3</v>
       </c>
       <c r="B46" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C46" t="s">
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E46" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="13">
@@ -1578,13 +1572,13 @@
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C47" t="s">
         <v>2</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E47" t="s">
         <v>4</v>
@@ -1595,16 +1589,16 @@
         <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C48" t="s">
         <v>2</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E48" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="13">
@@ -1612,13 +1606,13 @@
         <v>2</v>
       </c>
       <c r="B49" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C49" t="s">
         <v>2</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E49" t="s">
         <v>4</v>
@@ -1629,16 +1623,16 @@
         <v>3</v>
       </c>
       <c r="B50" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E50" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="13">
@@ -1646,16 +1640,16 @@
         <v>3</v>
       </c>
       <c r="B51" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C51" t="s">
         <v>2</v>
       </c>
       <c r="D51" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E51" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="13">
@@ -1663,16 +1657,16 @@
         <v>3</v>
       </c>
       <c r="B52" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C52" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D52" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E52" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="13">
@@ -1680,16 +1674,16 @@
         <v>3</v>
       </c>
       <c r="B53" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C53" t="s">
         <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E53" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="13">
@@ -1697,16 +1691,16 @@
         <v>2</v>
       </c>
       <c r="B54" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C54" t="s">
         <v>2</v>
       </c>
       <c r="D54" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E54" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="13">
@@ -1714,16 +1708,16 @@
         <v>2</v>
       </c>
       <c r="B55" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C55" t="s">
         <v>2</v>
       </c>
       <c r="D55" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="E55" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="13">
@@ -1731,16 +1725,16 @@
         <v>3</v>
       </c>
       <c r="B56" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C56" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D56" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E56" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="13">
@@ -1748,16 +1742,16 @@
         <v>3</v>
       </c>
       <c r="B57" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C57" t="s">
         <v>2</v>
       </c>
       <c r="D57" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E57" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="13">
@@ -1765,13 +1759,13 @@
         <v>2</v>
       </c>
       <c r="B58" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C58" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D58" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E58" t="s">
         <v>4</v>
@@ -1782,16 +1776,16 @@
         <v>1</v>
       </c>
       <c r="B59" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C59" t="s">
         <v>2</v>
       </c>
       <c r="D59" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="E59" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="13">
@@ -1799,16 +1793,16 @@
         <v>2</v>
       </c>
       <c r="B60" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C60" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E60" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="13">
@@ -1816,13 +1810,13 @@
         <v>2</v>
       </c>
       <c r="B61" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C61" t="s">
         <v>2</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E61" t="s">
         <v>4</v>
@@ -1833,16 +1827,16 @@
         <v>3</v>
       </c>
       <c r="B62" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C62" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D62" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E62" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="13">
@@ -1850,16 +1844,16 @@
         <v>2</v>
       </c>
       <c r="B63" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C63" t="s">
         <v>2</v>
       </c>
       <c r="D63" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E63" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="13">
@@ -1867,16 +1861,16 @@
         <v>1</v>
       </c>
       <c r="B64" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C64" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D64" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E64" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="13">
@@ -1884,16 +1878,16 @@
         <v>3</v>
       </c>
       <c r="B65" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C65" t="s">
         <v>2</v>
       </c>
       <c r="D65" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E65" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="13">
@@ -1901,16 +1895,16 @@
         <v>1</v>
       </c>
       <c r="B66" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C66" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E66" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="13">
@@ -1918,16 +1912,16 @@
         <v>1</v>
       </c>
       <c r="B67" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C67" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D67" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E67" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="13">

</xml_diff>